<commit_message>
Updated code and bug fixes, Release R01.00.23-20150211
</commit_message>
<xml_diff>
--- a/FrontEndChanges.xlsx
+++ b/FrontEndChanges.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Scripts</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 'X merge.js' in col D : Previously overrode, but no longer overriding</t>
+  </si>
+  <si>
+    <t>aspx to xhtml line 113</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code and bug fixes, Release R01.00.58-20150625
</commit_message>
<xml_diff>
--- a/FrontEndChanges.xlsx
+++ b/FrontEndChanges.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Scripts</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>aspx to xhtml line 113</t>
+  </si>
+  <si>
+    <t>TestShell/Modules/audit.js</t>
+  </si>
+  <si>
+    <t>Commented out line 106-116, timer task of audit is not implemented on server side</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,6 +791,14 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>